<commit_message>
final recipes for version 2 MMFD release
</commit_message>
<xml_diff>
--- a/src/gap_fill_met_city.xlsx
+++ b/src/gap_fill_met_city.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dcsewall\code\SCMStandz\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\root\code\SCMStandz\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306D4871-0D77-4381-A573-15DAB3C0D420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6365B92-0B94-4F62-BDE4-C0DCE52C866A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1125" yWindow="1125" windowWidth="28080" windowHeight="15945" xr2:uid="{339A30FB-E7B8-4ED3-846D-C9E4868AB851}"/>
   </bookViews>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="67">
   <si>
     <t>param</t>
   </si>
@@ -216,6 +205,27 @@
   </si>
   <si>
     <t>20200714 05:35</t>
+  </si>
+  <si>
+    <t>lat_tower</t>
+  </si>
+  <si>
+    <t>lon_tower</t>
+  </si>
+  <si>
+    <t>zenith_true</t>
+  </si>
+  <si>
+    <t>20191015 00:00</t>
+  </si>
+  <si>
+    <t>20200426 11:31</t>
+  </si>
+  <si>
+    <t>20200426 11:55</t>
+  </si>
+  <si>
+    <t>20191024 05:29</t>
   </si>
 </sst>
 </file>
@@ -256,11 +266,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,16 +587,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{743DC658-9119-48D6-9B2D-806F7D963900}">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -606,16 +619,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
+        <v>49</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -623,13 +636,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
+        <v>62</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="D3" t="s">
         <v>53</v>
@@ -640,7 +653,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -657,10 +670,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -674,10 +687,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -691,13 +704,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
         <v>53</v>
@@ -708,13 +721,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
         <v>53</v>
@@ -725,7 +738,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>11</v>
@@ -742,7 +755,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
@@ -759,7 +772,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
@@ -776,41 +789,41 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
         <v>53</v>
       </c>
       <c r="E12">
-        <v>-600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
         <v>53</v>
       </c>
       <c r="E13">
-        <v>-600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
@@ -827,13 +840,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
         <v>53</v>
@@ -844,13 +857,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
         <v>53</v>
@@ -861,41 +874,41 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D17" t="s">
         <v>53</v>
       </c>
       <c r="E17">
-        <v>1654</v>
+        <v>-600</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D18" t="s">
         <v>53</v>
       </c>
       <c r="E18">
-        <v>1654</v>
+        <v>-600</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
@@ -912,10 +925,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
         <v>19</v>
@@ -929,10 +942,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
         <v>19</v>
@@ -946,41 +959,41 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" t="s">
         <v>53</v>
       </c>
       <c r="E22">
-        <v>-4238</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D23" t="s">
         <v>53</v>
       </c>
       <c r="E23">
-        <v>-4238</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
         <v>22</v>
@@ -997,10 +1010,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
         <v>20</v>
@@ -1014,10 +1027,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
         <v>20</v>
@@ -1031,41 +1044,41 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C27" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D27" t="s">
         <v>53</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>-4238</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C28" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D28" t="s">
         <v>53</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>-4238</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="B29" t="s">
         <v>23</v>
@@ -1082,7 +1095,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B30" t="s">
         <v>23</v>
@@ -1099,7 +1112,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s">
         <v>23</v>
@@ -1116,13 +1129,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D32" t="s">
         <v>53</v>
@@ -1133,13 +1146,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D33" t="s">
         <v>53</v>
@@ -1150,7 +1163,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="B34" t="s">
         <v>26</v>
@@ -1167,7 +1180,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B35" t="s">
         <v>26</v>
@@ -1184,7 +1197,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
         <v>26</v>
@@ -1201,16 +1214,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C37" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -1218,16 +1231,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C38" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -1235,7 +1248,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="B39" t="s">
         <v>27</v>
@@ -1252,7 +1265,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B40" t="s">
         <v>27</v>
@@ -1269,7 +1282,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
         <v>27</v>
@@ -1286,16 +1299,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D42" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -1303,16 +1316,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D43" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -1320,13 +1333,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="B44" t="s">
         <v>30</v>
       </c>
       <c r="C44" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D44" t="s">
         <v>53</v>
@@ -1337,7 +1350,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B45" t="s">
         <v>30</v>
@@ -1354,13 +1367,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B46" t="s">
         <v>30</v>
       </c>
       <c r="C46" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D46" t="s">
         <v>53</v>
@@ -1371,16 +1384,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B47" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C47" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -1388,16 +1401,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C48" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -1405,7 +1418,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="B49" t="s">
         <v>33</v>
@@ -1422,7 +1435,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B50" t="s">
         <v>33</v>
@@ -1439,7 +1452,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B51" t="s">
         <v>33</v>
@@ -1456,16 +1469,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C52" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E52">
         <v>0</v>
@@ -1473,16 +1486,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C53" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -1490,7 +1503,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="B54" t="s">
         <v>34</v>
@@ -1507,13 +1520,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="B55" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C55" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D55" t="s">
         <v>55</v>
@@ -1524,13 +1537,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="B56" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C56" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D56" t="s">
         <v>55</v>
@@ -1541,13 +1554,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B57" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C57" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D57" t="s">
         <v>55</v>
@@ -1558,13 +1571,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B58" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C58" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D58" t="s">
         <v>55</v>
@@ -1575,7 +1588,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B59" t="s">
         <v>39</v>
@@ -1592,7 +1605,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="B60" t="s">
         <v>39</v>
@@ -1609,13 +1622,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="B61" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C61" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D61" t="s">
         <v>55</v>
@@ -1626,13 +1639,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="B62" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C62" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D62" t="s">
         <v>55</v>
@@ -1643,13 +1656,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="B63" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C63" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D63" t="s">
         <v>55</v>
@@ -1660,16 +1673,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>6</v>
-      </c>
-      <c r="B64" t="s">
-        <v>43</v>
-      </c>
-      <c r="C64" t="s">
-        <v>41</v>
+        <v>49</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="D64" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -1677,10 +1690,10 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B65" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C65" t="s">
         <v>41</v>
@@ -1694,13 +1707,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="B66" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C66" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D66" t="s">
         <v>55</v>
@@ -1711,13 +1724,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B67" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C67" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D67" t="s">
         <v>55</v>
@@ -1728,13 +1741,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="B68" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C68" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D68" t="s">
         <v>55</v>
@@ -1745,13 +1758,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B69" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C69" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D69" t="s">
         <v>55</v>
@@ -1762,13 +1775,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="B70" t="s">
         <v>44</v>
       </c>
       <c r="C70" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D70" t="s">
         <v>55</v>
@@ -1779,13 +1792,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B71" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C71" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D71" t="s">
         <v>55</v>
@@ -1796,13 +1809,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="B72" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C72" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D72" t="s">
         <v>55</v>
@@ -1813,13 +1826,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B73" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C73" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D73" t="s">
         <v>55</v>
@@ -1830,20 +1843,147 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>52</v>
+      </c>
+      <c r="B74" t="s">
+        <v>44</v>
+      </c>
+      <c r="C74" t="s">
+        <v>45</v>
+      </c>
+      <c r="D74" t="s">
+        <v>55</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" t="s">
+        <v>44</v>
+      </c>
+      <c r="C75" t="s">
+        <v>47</v>
+      </c>
+      <c r="D75" t="s">
+        <v>55</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>7</v>
+      </c>
+      <c r="B76" t="s">
+        <v>44</v>
+      </c>
+      <c r="C76" t="s">
+        <v>47</v>
+      </c>
+      <c r="D76" t="s">
+        <v>55</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>49</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B77" t="s">
+        <v>48</v>
+      </c>
+      <c r="C77" t="s">
+        <v>50</v>
+      </c>
+      <c r="D77" t="s">
+        <v>55</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>35</v>
+      </c>
+      <c r="B78" t="s">
+        <v>48</v>
+      </c>
+      <c r="C78" t="s">
+        <v>46</v>
+      </c>
+      <c r="D78" t="s">
+        <v>55</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>62</v>
+      </c>
+      <c r="B79" t="s">
+        <v>48</v>
+      </c>
+      <c r="C79" t="s">
+        <v>45</v>
+      </c>
+      <c r="D79" t="s">
+        <v>55</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>49</v>
+      </c>
+      <c r="B80" t="s">
+        <v>57</v>
+      </c>
+      <c r="C80" t="s">
+        <v>58</v>
+      </c>
+      <c r="D80" t="s">
+        <v>55</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>49</v>
+      </c>
+      <c r="B81" t="s">
         <v>59</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C81" t="s">
         <v>56</v>
       </c>
-      <c r="D74" t="s">
-        <v>55</v>
-      </c>
-      <c r="E74">
-        <v>0</v>
-      </c>
+      <c r="D81" t="s">
+        <v>55</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>